<commit_message>
Added output file command line option
</commit_message>
<xml_diff>
--- a/24Team4JudgingRooms.xlsx
+++ b/24Team4JudgingRooms.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/blfarrel/Documents/code/wifllscheduler/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEC7783C-437D-4B4B-BA9F-5834D60306A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{814DECBF-8F57-7142-9D6E-81E20A69E91B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17660" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="14" r:id="rId1"/>
@@ -61,7 +61,7 @@
     <definedName name="PMRemainingMatches">MOD(PMTEAMS,(NumberOfTablePairs*2))</definedName>
     <definedName name="PMTEAMS">HalfList</definedName>
     <definedName name="PMWildCardMatches" comment="=MOD((NumberOfTablePairs*2)-PMRemainingMatches,(NumberOfTablePairs*2))">MOD((NumberOfTablePairs*2)-PMRemainingMatches,(NumberOfTablePairs*2))</definedName>
-    <definedName name="TableColors">TournamentSetup!$G$25:$G$28</definedName>
+    <definedName name="TableColors">TournamentSetup!$E$35:$E$38</definedName>
     <definedName name="TablePattern">TournamentSetup!$L$4</definedName>
     <definedName name="TableTimeRd1Offset">INDEX(_xlfn.CHOOSECOLS(INDIRECT(TablePattern),3), MATCH(INDIRECT(ADDRESS(ROW(),5,1,1)),_xlfn.CHOOSECOLS(INDIRECT(TablePattern),4),0))</definedName>
     <definedName name="TableTimeRd2Offset">INDEX(_xlfn.CHOOSECOLS(INDIRECT(TablePattern),3), MATCH(INDIRECT(ADDRESS(ROW(),7,1,1)),_xlfn.CHOOSECOLS(INDIRECT(TablePattern),4),0))</definedName>
@@ -746,9 +746,6 @@
     <t>Coach 23</t>
   </si>
   <si>
-    <t>Team 24</t>
-  </si>
-  <si>
     <t>Coach 24</t>
   </si>
   <si>
@@ -861,6 +858,9 @@
   </si>
   <si>
     <t>Practice round start time 1</t>
+  </si>
+  <si>
+    <t>Team 24</t>
   </si>
 </sst>
 </file>
@@ -975,7 +975,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -1004,6 +1004,13 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="2"/>
     <xf numFmtId="14" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -1025,15 +1032,6 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -1438,251 +1436,251 @@
       <c r="A5" s="6" t="s">
         <v>119</v>
       </c>
-      <c r="B5" s="22" t="s">
+      <c r="B5" s="25" t="s">
         <v>120</v>
       </c>
-      <c r="C5" s="22"/>
-      <c r="D5" s="22"/>
-      <c r="E5" s="22"/>
-      <c r="F5" s="22"/>
-      <c r="G5" s="22"/>
-      <c r="H5" s="22"/>
-      <c r="I5" s="22"/>
-      <c r="J5" s="22"/>
-      <c r="K5" s="22"/>
-      <c r="L5" s="22"/>
-      <c r="M5" s="22"/>
-      <c r="N5" s="22"/>
-      <c r="O5" s="22"/>
-      <c r="P5" s="22"/>
+      <c r="C5" s="25"/>
+      <c r="D5" s="25"/>
+      <c r="E5" s="25"/>
+      <c r="F5" s="25"/>
+      <c r="G5" s="25"/>
+      <c r="H5" s="25"/>
+      <c r="I5" s="25"/>
+      <c r="J5" s="25"/>
+      <c r="K5" s="25"/>
+      <c r="L5" s="25"/>
+      <c r="M5" s="25"/>
+      <c r="N5" s="25"/>
+      <c r="O5" s="25"/>
+      <c r="P5" s="25"/>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A6" s="24" t="s">
+      <c r="A6" s="27" t="s">
         <v>121</v>
       </c>
-      <c r="B6" s="23" t="s">
+      <c r="B6" s="26" t="s">
         <v>122</v>
       </c>
-      <c r="C6" s="23"/>
-      <c r="D6" s="23"/>
-      <c r="E6" s="23"/>
-      <c r="F6" s="23"/>
-      <c r="G6" s="23"/>
-      <c r="H6" s="23"/>
-      <c r="I6" s="23"/>
-      <c r="J6" s="23"/>
-      <c r="K6" s="23"/>
-      <c r="L6" s="23"/>
-      <c r="M6" s="23"/>
-      <c r="N6" s="23"/>
-      <c r="O6" s="23"/>
-      <c r="P6" s="23"/>
+      <c r="C6" s="26"/>
+      <c r="D6" s="26"/>
+      <c r="E6" s="26"/>
+      <c r="F6" s="26"/>
+      <c r="G6" s="26"/>
+      <c r="H6" s="26"/>
+      <c r="I6" s="26"/>
+      <c r="J6" s="26"/>
+      <c r="K6" s="26"/>
+      <c r="L6" s="26"/>
+      <c r="M6" s="26"/>
+      <c r="N6" s="26"/>
+      <c r="O6" s="26"/>
+      <c r="P6" s="26"/>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A7" s="24"/>
-      <c r="B7" s="23"/>
-      <c r="C7" s="23"/>
-      <c r="D7" s="23"/>
-      <c r="E7" s="23"/>
-      <c r="F7" s="23"/>
-      <c r="G7" s="23"/>
-      <c r="H7" s="23"/>
-      <c r="I7" s="23"/>
-      <c r="J7" s="23"/>
-      <c r="K7" s="23"/>
-      <c r="L7" s="23"/>
-      <c r="M7" s="23"/>
-      <c r="N7" s="23"/>
-      <c r="O7" s="23"/>
-      <c r="P7" s="23"/>
+      <c r="A7" s="27"/>
+      <c r="B7" s="26"/>
+      <c r="C7" s="26"/>
+      <c r="D7" s="26"/>
+      <c r="E7" s="26"/>
+      <c r="F7" s="26"/>
+      <c r="G7" s="26"/>
+      <c r="H7" s="26"/>
+      <c r="I7" s="26"/>
+      <c r="J7" s="26"/>
+      <c r="K7" s="26"/>
+      <c r="L7" s="26"/>
+      <c r="M7" s="26"/>
+      <c r="N7" s="26"/>
+      <c r="O7" s="26"/>
+      <c r="P7" s="26"/>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A8" s="24"/>
-      <c r="B8" s="23"/>
-      <c r="C8" s="23"/>
-      <c r="D8" s="23"/>
-      <c r="E8" s="23"/>
-      <c r="F8" s="23"/>
-      <c r="G8" s="23"/>
-      <c r="H8" s="23"/>
-      <c r="I8" s="23"/>
-      <c r="J8" s="23"/>
-      <c r="K8" s="23"/>
-      <c r="L8" s="23"/>
-      <c r="M8" s="23"/>
-      <c r="N8" s="23"/>
-      <c r="O8" s="23"/>
-      <c r="P8" s="23"/>
+      <c r="A8" s="27"/>
+      <c r="B8" s="26"/>
+      <c r="C8" s="26"/>
+      <c r="D8" s="26"/>
+      <c r="E8" s="26"/>
+      <c r="F8" s="26"/>
+      <c r="G8" s="26"/>
+      <c r="H8" s="26"/>
+      <c r="I8" s="26"/>
+      <c r="J8" s="26"/>
+      <c r="K8" s="26"/>
+      <c r="L8" s="26"/>
+      <c r="M8" s="26"/>
+      <c r="N8" s="26"/>
+      <c r="O8" s="26"/>
+      <c r="P8" s="26"/>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A9" s="24"/>
-      <c r="B9" s="23"/>
-      <c r="C9" s="23"/>
-      <c r="D9" s="23"/>
-      <c r="E9" s="23"/>
-      <c r="F9" s="23"/>
-      <c r="G9" s="23"/>
-      <c r="H9" s="23"/>
-      <c r="I9" s="23"/>
-      <c r="J9" s="23"/>
-      <c r="K9" s="23"/>
-      <c r="L9" s="23"/>
-      <c r="M9" s="23"/>
-      <c r="N9" s="23"/>
-      <c r="O9" s="23"/>
-      <c r="P9" s="23"/>
+      <c r="A9" s="27"/>
+      <c r="B9" s="26"/>
+      <c r="C9" s="26"/>
+      <c r="D9" s="26"/>
+      <c r="E9" s="26"/>
+      <c r="F9" s="26"/>
+      <c r="G9" s="26"/>
+      <c r="H9" s="26"/>
+      <c r="I9" s="26"/>
+      <c r="J9" s="26"/>
+      <c r="K9" s="26"/>
+      <c r="L9" s="26"/>
+      <c r="M9" s="26"/>
+      <c r="N9" s="26"/>
+      <c r="O9" s="26"/>
+      <c r="P9" s="26"/>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A10" s="24" t="s">
+      <c r="A10" s="27" t="s">
         <v>123</v>
       </c>
-      <c r="B10" s="24" t="s">
+      <c r="B10" s="27" t="s">
         <v>124</v>
       </c>
-      <c r="C10" s="24"/>
-      <c r="D10" s="24"/>
-      <c r="E10" s="24"/>
-      <c r="F10" s="24"/>
-      <c r="G10" s="24"/>
-      <c r="H10" s="24"/>
-      <c r="I10" s="24"/>
-      <c r="J10" s="24"/>
-      <c r="K10" s="24"/>
-      <c r="L10" s="24"/>
-      <c r="M10" s="24"/>
-      <c r="N10" s="24"/>
-      <c r="O10" s="24"/>
-      <c r="P10" s="24"/>
+      <c r="C10" s="27"/>
+      <c r="D10" s="27"/>
+      <c r="E10" s="27"/>
+      <c r="F10" s="27"/>
+      <c r="G10" s="27"/>
+      <c r="H10" s="27"/>
+      <c r="I10" s="27"/>
+      <c r="J10" s="27"/>
+      <c r="K10" s="27"/>
+      <c r="L10" s="27"/>
+      <c r="M10" s="27"/>
+      <c r="N10" s="27"/>
+      <c r="O10" s="27"/>
+      <c r="P10" s="27"/>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A11" s="24"/>
-      <c r="B11" s="24"/>
-      <c r="C11" s="24"/>
-      <c r="D11" s="24"/>
-      <c r="E11" s="24"/>
-      <c r="F11" s="24"/>
-      <c r="G11" s="24"/>
-      <c r="H11" s="24"/>
-      <c r="I11" s="24"/>
-      <c r="J11" s="24"/>
-      <c r="K11" s="24"/>
-      <c r="L11" s="24"/>
-      <c r="M11" s="24"/>
-      <c r="N11" s="24"/>
-      <c r="O11" s="24"/>
-      <c r="P11" s="24"/>
+      <c r="A11" s="27"/>
+      <c r="B11" s="27"/>
+      <c r="C11" s="27"/>
+      <c r="D11" s="27"/>
+      <c r="E11" s="27"/>
+      <c r="F11" s="27"/>
+      <c r="G11" s="27"/>
+      <c r="H11" s="27"/>
+      <c r="I11" s="27"/>
+      <c r="J11" s="27"/>
+      <c r="K11" s="27"/>
+      <c r="L11" s="27"/>
+      <c r="M11" s="27"/>
+      <c r="N11" s="27"/>
+      <c r="O11" s="27"/>
+      <c r="P11" s="27"/>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A12" s="24"/>
-      <c r="B12" s="24"/>
-      <c r="C12" s="24"/>
-      <c r="D12" s="24"/>
-      <c r="E12" s="24"/>
-      <c r="F12" s="24"/>
-      <c r="G12" s="24"/>
-      <c r="H12" s="24"/>
-      <c r="I12" s="24"/>
-      <c r="J12" s="24"/>
-      <c r="K12" s="24"/>
-      <c r="L12" s="24"/>
-      <c r="M12" s="24"/>
-      <c r="N12" s="24"/>
-      <c r="O12" s="24"/>
-      <c r="P12" s="24"/>
+      <c r="A12" s="27"/>
+      <c r="B12" s="27"/>
+      <c r="C12" s="27"/>
+      <c r="D12" s="27"/>
+      <c r="E12" s="27"/>
+      <c r="F12" s="27"/>
+      <c r="G12" s="27"/>
+      <c r="H12" s="27"/>
+      <c r="I12" s="27"/>
+      <c r="J12" s="27"/>
+      <c r="K12" s="27"/>
+      <c r="L12" s="27"/>
+      <c r="M12" s="27"/>
+      <c r="N12" s="27"/>
+      <c r="O12" s="27"/>
+      <c r="P12" s="27"/>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A13" s="24"/>
-      <c r="B13" s="24"/>
-      <c r="C13" s="24"/>
-      <c r="D13" s="24"/>
-      <c r="E13" s="24"/>
-      <c r="F13" s="24"/>
-      <c r="G13" s="24"/>
-      <c r="H13" s="24"/>
-      <c r="I13" s="24"/>
-      <c r="J13" s="24"/>
-      <c r="K13" s="24"/>
-      <c r="L13" s="24"/>
-      <c r="M13" s="24"/>
-      <c r="N13" s="24"/>
-      <c r="O13" s="24"/>
-      <c r="P13" s="24"/>
+      <c r="A13" s="27"/>
+      <c r="B13" s="27"/>
+      <c r="C13" s="27"/>
+      <c r="D13" s="27"/>
+      <c r="E13" s="27"/>
+      <c r="F13" s="27"/>
+      <c r="G13" s="27"/>
+      <c r="H13" s="27"/>
+      <c r="I13" s="27"/>
+      <c r="J13" s="27"/>
+      <c r="K13" s="27"/>
+      <c r="L13" s="27"/>
+      <c r="M13" s="27"/>
+      <c r="N13" s="27"/>
+      <c r="O13" s="27"/>
+      <c r="P13" s="27"/>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A14" s="23" t="s">
+      <c r="A14" s="26" t="s">
         <v>125</v>
       </c>
-      <c r="B14" s="24" t="s">
+      <c r="B14" s="27" t="s">
         <v>126</v>
       </c>
-      <c r="C14" s="24"/>
-      <c r="D14" s="24"/>
-      <c r="E14" s="24"/>
-      <c r="F14" s="24"/>
-      <c r="G14" s="24"/>
-      <c r="H14" s="24"/>
-      <c r="I14" s="24"/>
-      <c r="J14" s="24"/>
-      <c r="K14" s="24"/>
-      <c r="L14" s="24"/>
-      <c r="M14" s="24"/>
-      <c r="N14" s="24"/>
-      <c r="O14" s="24"/>
-      <c r="P14" s="24"/>
+      <c r="C14" s="27"/>
+      <c r="D14" s="27"/>
+      <c r="E14" s="27"/>
+      <c r="F14" s="27"/>
+      <c r="G14" s="27"/>
+      <c r="H14" s="27"/>
+      <c r="I14" s="27"/>
+      <c r="J14" s="27"/>
+      <c r="K14" s="27"/>
+      <c r="L14" s="27"/>
+      <c r="M14" s="27"/>
+      <c r="N14" s="27"/>
+      <c r="O14" s="27"/>
+      <c r="P14" s="27"/>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A15" s="23"/>
-      <c r="B15" s="24"/>
-      <c r="C15" s="24"/>
-      <c r="D15" s="24"/>
-      <c r="E15" s="24"/>
-      <c r="F15" s="24"/>
-      <c r="G15" s="24"/>
-      <c r="H15" s="24"/>
-      <c r="I15" s="24"/>
-      <c r="J15" s="24"/>
-      <c r="K15" s="24"/>
-      <c r="L15" s="24"/>
-      <c r="M15" s="24"/>
-      <c r="N15" s="24"/>
-      <c r="O15" s="24"/>
-      <c r="P15" s="24"/>
+      <c r="A15" s="26"/>
+      <c r="B15" s="27"/>
+      <c r="C15" s="27"/>
+      <c r="D15" s="27"/>
+      <c r="E15" s="27"/>
+      <c r="F15" s="27"/>
+      <c r="G15" s="27"/>
+      <c r="H15" s="27"/>
+      <c r="I15" s="27"/>
+      <c r="J15" s="27"/>
+      <c r="K15" s="27"/>
+      <c r="L15" s="27"/>
+      <c r="M15" s="27"/>
+      <c r="N15" s="27"/>
+      <c r="O15" s="27"/>
+      <c r="P15" s="27"/>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A16" s="23"/>
-      <c r="B16" s="24"/>
-      <c r="C16" s="24"/>
-      <c r="D16" s="24"/>
-      <c r="E16" s="24"/>
-      <c r="F16" s="24"/>
-      <c r="G16" s="24"/>
-      <c r="H16" s="24"/>
-      <c r="I16" s="24"/>
-      <c r="J16" s="24"/>
-      <c r="K16" s="24"/>
-      <c r="L16" s="24"/>
-      <c r="M16" s="24"/>
-      <c r="N16" s="24"/>
-      <c r="O16" s="24"/>
-      <c r="P16" s="24"/>
+      <c r="A16" s="26"/>
+      <c r="B16" s="27"/>
+      <c r="C16" s="27"/>
+      <c r="D16" s="27"/>
+      <c r="E16" s="27"/>
+      <c r="F16" s="27"/>
+      <c r="G16" s="27"/>
+      <c r="H16" s="27"/>
+      <c r="I16" s="27"/>
+      <c r="J16" s="27"/>
+      <c r="K16" s="27"/>
+      <c r="L16" s="27"/>
+      <c r="M16" s="27"/>
+      <c r="N16" s="27"/>
+      <c r="O16" s="27"/>
+      <c r="P16" s="27"/>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A17" s="23"/>
-      <c r="B17" s="24"/>
-      <c r="C17" s="24"/>
-      <c r="D17" s="24"/>
-      <c r="E17" s="24"/>
-      <c r="F17" s="24"/>
-      <c r="G17" s="24"/>
-      <c r="H17" s="24"/>
-      <c r="I17" s="24"/>
-      <c r="J17" s="24"/>
-      <c r="K17" s="24"/>
-      <c r="L17" s="24"/>
-      <c r="M17" s="24"/>
-      <c r="N17" s="24"/>
-      <c r="O17" s="24"/>
-      <c r="P17" s="24"/>
+      <c r="A17" s="26"/>
+      <c r="B17" s="27"/>
+      <c r="C17" s="27"/>
+      <c r="D17" s="27"/>
+      <c r="E17" s="27"/>
+      <c r="F17" s="27"/>
+      <c r="G17" s="27"/>
+      <c r="H17" s="27"/>
+      <c r="I17" s="27"/>
+      <c r="J17" s="27"/>
+      <c r="K17" s="27"/>
+      <c r="L17" s="27"/>
+      <c r="M17" s="27"/>
+      <c r="N17" s="27"/>
+      <c r="O17" s="27"/>
+      <c r="P17" s="27"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -1703,13 +1701,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0C4C8D7-0378-4227-AF78-04162F519C92}">
   <dimension ref="A1:R61"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E36" sqref="E36"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24:C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="16.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.2">
@@ -1765,7 +1764,7 @@
     <row r="2" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A2">
         <f t="shared" ref="A2:A61" ca="1" si="0">RAND()</f>
-        <v>8.969620691154967E-2</v>
+        <v>0.87001161974676011</v>
       </c>
       <c r="B2" s="2">
         <v>1</v>
@@ -1797,7 +1796,7 @@
     <row r="3" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A3">
         <f t="shared" ca="1" si="0"/>
-        <v>0.50332928056707915</v>
+        <v>4.820037806882671E-2</v>
       </c>
       <c r="B3" s="2">
         <v>2</v>
@@ -1829,7 +1828,7 @@
     <row r="4" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.61150349943838322</v>
+        <v>9.764874127947587E-2</v>
       </c>
       <c r="B4" s="2">
         <v>3</v>
@@ -1858,7 +1857,7 @@
     <row r="5" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A5">
         <f t="shared" ca="1" si="0"/>
-        <v>0.51221878391754116</v>
+        <v>0.77648005363054595</v>
       </c>
       <c r="B5" s="2">
         <v>4</v>
@@ -1880,7 +1879,7 @@
     <row r="6" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A6">
         <f t="shared" ca="1" si="0"/>
-        <v>0.19728453224241915</v>
+        <v>0.72597214219454032</v>
       </c>
       <c r="B6" s="2">
         <v>5</v>
@@ -1902,7 +1901,7 @@
     <row r="7" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A7">
         <f t="shared" ca="1" si="0"/>
-        <v>6.8004188121948195E-2</v>
+        <v>0.48095072196960409</v>
       </c>
       <c r="B7" s="2">
         <v>6</v>
@@ -1924,7 +1923,7 @@
     <row r="8" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A8">
         <f t="shared" ca="1" si="0"/>
-        <v>0.85692188529915625</v>
+        <v>0.80054058811889039</v>
       </c>
       <c r="B8" s="2">
         <v>7</v>
@@ -1945,7 +1944,7 @@
     <row r="9" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A9">
         <f t="shared" ca="1" si="0"/>
-        <v>2.9381977408869608E-2</v>
+        <v>0.94226013304675993</v>
       </c>
       <c r="B9" s="2">
         <v>8</v>
@@ -1966,7 +1965,7 @@
     <row r="10" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A10">
         <f t="shared" ca="1" si="0"/>
-        <v>0.41407511047765211</v>
+        <v>0.7945330265212831</v>
       </c>
       <c r="B10" s="2">
         <v>9</v>
@@ -1987,7 +1986,7 @@
     <row r="11" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A11">
         <f t="shared" ca="1" si="0"/>
-        <v>0.41501449199962337</v>
+        <v>0.37471568695871427</v>
       </c>
       <c r="B11" s="2">
         <v>10</v>
@@ -2008,7 +2007,7 @@
     <row r="12" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A12">
         <f t="shared" ca="1" si="0"/>
-        <v>0.11428561719179509</v>
+        <v>0.32770804949583332</v>
       </c>
       <c r="B12" s="2">
         <v>11</v>
@@ -2029,7 +2028,7 @@
     <row r="13" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A13">
         <f t="shared" ca="1" si="0"/>
-        <v>0.6169899778947765</v>
+        <v>0.85216300184181271</v>
       </c>
       <c r="B13" s="2">
         <v>12</v>
@@ -2050,7 +2049,7 @@
     <row r="14" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A14">
         <f t="shared" ca="1" si="0"/>
-        <v>0.52593207032210587</v>
+        <v>0.93655343119750134</v>
       </c>
       <c r="B14" s="2">
         <v>13</v>
@@ -2071,7 +2070,7 @@
     <row r="15" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A15">
         <f t="shared" ca="1" si="0"/>
-        <v>0.43822542573539336</v>
+        <v>0.55198013021285397</v>
       </c>
       <c r="B15" s="2">
         <v>14</v>
@@ -2092,7 +2091,7 @@
     <row r="16" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A16">
         <f t="shared" ca="1" si="0"/>
-        <v>0.66824109068459059</v>
+        <v>0.5117016480546277</v>
       </c>
       <c r="B16" s="2">
         <v>15</v>
@@ -2113,7 +2112,7 @@
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17">
         <f t="shared" ca="1" si="0"/>
-        <v>0.69602690234259723</v>
+        <v>0.80544131191297608</v>
       </c>
       <c r="B17" s="2">
         <v>16</v>
@@ -2134,7 +2133,7 @@
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18">
         <f t="shared" ca="1" si="0"/>
-        <v>0.70176662181492822</v>
+        <v>0.6628883432811512</v>
       </c>
       <c r="B18" s="2">
         <v>17</v>
@@ -2155,7 +2154,7 @@
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19">
         <f t="shared" ca="1" si="0"/>
-        <v>0.32437787486385594</v>
+        <v>0.80250075358196626</v>
       </c>
       <c r="B19" s="2">
         <v>18</v>
@@ -2176,7 +2175,7 @@
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20">
         <f t="shared" ca="1" si="0"/>
-        <v>0.9672342430189611</v>
+        <v>0.88762158133118951</v>
       </c>
       <c r="B20" s="2">
         <v>19</v>
@@ -2197,7 +2196,7 @@
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21">
         <f t="shared" ca="1" si="0"/>
-        <v>0.93313412003278484</v>
+        <v>0.98073167414061824</v>
       </c>
       <c r="B21" s="2">
         <v>20</v>
@@ -2218,7 +2217,7 @@
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22">
         <f t="shared" ca="1" si="0"/>
-        <v>0.30590951183292336</v>
+        <v>0.82043415384586882</v>
       </c>
       <c r="B22" s="2">
         <v>21</v>
@@ -2239,7 +2238,7 @@
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23">
         <f t="shared" ca="1" si="0"/>
-        <v>0.5092750698871723</v>
+        <v>0.1017827722381841</v>
       </c>
       <c r="B23" s="2">
         <v>22</v>
@@ -2260,7 +2259,7 @@
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24">
         <f t="shared" ca="1" si="0"/>
-        <v>0.3900419817182128</v>
+        <v>0.33377552733241256</v>
       </c>
       <c r="B24" s="2">
         <v>23</v>
@@ -2281,13 +2280,13 @@
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25">
         <f t="shared" ca="1" si="0"/>
-        <v>0.10186589107205102</v>
+        <v>3.820334420990823E-2</v>
       </c>
       <c r="B25" s="2">
         <v>24</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>140</v>
+        <v>178</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>20</v>
@@ -2296,13 +2295,13 @@
         <v>17</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26">
         <f t="shared" ca="1" si="0"/>
-        <v>0.85133991747544624</v>
+        <v>0.11136439730773029</v>
       </c>
       <c r="B26" s="2"/>
       <c r="C26" s="1"/>
@@ -2313,7 +2312,7 @@
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27">
         <f t="shared" ca="1" si="0"/>
-        <v>0.46709730790987181</v>
+        <v>0.59066004098654756</v>
       </c>
       <c r="B27" s="2"/>
       <c r="C27" s="1"/>
@@ -2324,7 +2323,7 @@
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28">
         <f t="shared" ca="1" si="0"/>
-        <v>7.7609256533890392E-2</v>
+        <v>0.62141328759432601</v>
       </c>
       <c r="B28" s="2"/>
       <c r="C28" s="1"/>
@@ -2335,7 +2334,7 @@
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29">
         <f t="shared" ca="1" si="0"/>
-        <v>0.12231682227658891</v>
+        <v>0.44757368164566003</v>
       </c>
       <c r="B29" s="2"/>
       <c r="C29" s="1"/>
@@ -2346,7 +2345,7 @@
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30">
         <f t="shared" ca="1" si="0"/>
-        <v>6.6318514569662868E-2</v>
+        <v>0.32687830525989248</v>
       </c>
       <c r="B30" s="2"/>
       <c r="C30" s="1"/>
@@ -2357,19 +2356,19 @@
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31">
         <f t="shared" ca="1" si="0"/>
-        <v>1.2353883956619183E-2</v>
+        <v>0.72524960833574692</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32">
         <f t="shared" ca="1" si="0"/>
-        <v>0.30157551344229205</v>
+        <v>0.54466334460683463</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33">
         <f t="shared" ca="1" si="0"/>
-        <v>0.30508812100702187</v>
+        <v>0.67634380459342169</v>
       </c>
       <c r="B33" s="2"/>
       <c r="C33" s="1"/>
@@ -2380,7 +2379,7 @@
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34">
         <f t="shared" ca="1" si="0"/>
-        <v>0.22966956203167666</v>
+        <v>6.8999507679777472E-2</v>
       </c>
       <c r="B34" s="2"/>
       <c r="C34" s="1"/>
@@ -2391,7 +2390,7 @@
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35">
         <f t="shared" ca="1" si="0"/>
-        <v>0.25645975583209935</v>
+        <v>0.37276293064865951</v>
       </c>
       <c r="B35" s="2"/>
       <c r="C35" s="1"/>
@@ -2402,7 +2401,7 @@
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36">
         <f t="shared" ca="1" si="0"/>
-        <v>0.70672576422254729</v>
+        <v>0.6085848243217532</v>
       </c>
       <c r="B36" s="2"/>
       <c r="C36" s="1"/>
@@ -2413,7 +2412,7 @@
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37">
         <f t="shared" ca="1" si="0"/>
-        <v>2.8821539983041267E-2</v>
+        <v>7.4807520149076434E-2</v>
       </c>
       <c r="B37" s="2"/>
       <c r="C37" s="1"/>
@@ -2424,7 +2423,7 @@
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38">
         <f t="shared" ca="1" si="0"/>
-        <v>0.50023031121869044</v>
+        <v>0.20439028949298621</v>
       </c>
       <c r="B38" s="2"/>
       <c r="C38" s="1"/>
@@ -2435,7 +2434,7 @@
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39">
         <f t="shared" ca="1" si="0"/>
-        <v>0.61005320551907638</v>
+        <v>0.52765885079236685</v>
       </c>
       <c r="B39" s="2"/>
       <c r="C39" s="1"/>
@@ -2446,7 +2445,7 @@
     <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40">
         <f t="shared" ca="1" si="0"/>
-        <v>0.85669749287341523</v>
+        <v>0.78983434915333994</v>
       </c>
       <c r="B40" s="2"/>
       <c r="C40" s="1"/>
@@ -2457,7 +2456,7 @@
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41">
         <f t="shared" ca="1" si="0"/>
-        <v>0.99777070750310237</v>
+        <v>0.26654935413266001</v>
       </c>
       <c r="B41" s="2"/>
       <c r="C41" s="1"/>
@@ -2468,7 +2467,7 @@
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42">
         <f t="shared" ca="1" si="0"/>
-        <v>0.46575638435539191</v>
+        <v>0.50695480748473265</v>
       </c>
       <c r="B42" s="2"/>
       <c r="C42" s="1"/>
@@ -2479,7 +2478,7 @@
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43">
         <f t="shared" ca="1" si="0"/>
-        <v>0.33714308427187056</v>
+        <v>0.44007768862345653</v>
       </c>
       <c r="B43" s="2"/>
       <c r="C43" s="1"/>
@@ -2490,7 +2489,7 @@
     <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44">
         <f t="shared" ca="1" si="0"/>
-        <v>0.63902368702737133</v>
+        <v>0.63120541882908043</v>
       </c>
       <c r="B44" s="2"/>
       <c r="C44" s="1"/>
@@ -2501,7 +2500,7 @@
     <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45">
         <f t="shared" ca="1" si="0"/>
-        <v>0.27684539090167692</v>
+        <v>0.63597922091985759</v>
       </c>
       <c r="B45" s="2"/>
       <c r="C45" s="1"/>
@@ -2512,7 +2511,7 @@
     <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46">
         <f t="shared" ca="1" si="0"/>
-        <v>0.4112922240104625</v>
+        <v>0.84978236730738088</v>
       </c>
       <c r="B46" s="2"/>
       <c r="C46" s="1"/>
@@ -2523,7 +2522,7 @@
     <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47">
         <f t="shared" ca="1" si="0"/>
-        <v>0.70285196020872187</v>
+        <v>0.79305833264250503</v>
       </c>
       <c r="B47" s="2"/>
       <c r="C47" s="1"/>
@@ -2534,7 +2533,7 @@
     <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48">
         <f t="shared" ca="1" si="0"/>
-        <v>0.20848863521567229</v>
+        <v>0.67879381819529816</v>
       </c>
       <c r="B48" s="2"/>
       <c r="C48" s="1"/>
@@ -2545,7 +2544,7 @@
     <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49">
         <f t="shared" ca="1" si="0"/>
-        <v>0.234151244356959</v>
+        <v>0.28652033301494428</v>
       </c>
       <c r="B49" s="2"/>
       <c r="C49" s="1"/>
@@ -2556,7 +2555,7 @@
     <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50">
         <f t="shared" ca="1" si="0"/>
-        <v>0.80135061049946454</v>
+        <v>0.21063686905888368</v>
       </c>
       <c r="B50" s="2"/>
       <c r="C50" s="1"/>
@@ -2567,7 +2566,7 @@
     <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51">
         <f t="shared" ca="1" si="0"/>
-        <v>7.4310105019312012E-2</v>
+        <v>0.52751659774498438</v>
       </c>
       <c r="B51" s="2"/>
       <c r="C51" s="1"/>
@@ -2578,7 +2577,7 @@
     <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52">
         <f t="shared" ca="1" si="0"/>
-        <v>0.51939427318725184</v>
+        <v>3.6091592972389286E-2</v>
       </c>
       <c r="B52" s="2"/>
       <c r="C52" s="1"/>
@@ -2589,7 +2588,7 @@
     <row r="53" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A53">
         <f t="shared" ca="1" si="0"/>
-        <v>0.25955684255790679</v>
+        <v>8.9002306797734687E-2</v>
       </c>
       <c r="B53" s="2"/>
       <c r="C53" s="1"/>
@@ -2600,7 +2599,7 @@
     <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A54">
         <f t="shared" ca="1" si="0"/>
-        <v>0.12200288988621433</v>
+        <v>0.64567076272483315</v>
       </c>
       <c r="B54" s="2"/>
       <c r="C54" s="1"/>
@@ -2611,7 +2610,7 @@
     <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55">
         <f t="shared" ca="1" si="0"/>
-        <v>0.67876570777524226</v>
+        <v>0.29384395113538841</v>
       </c>
       <c r="B55" s="2"/>
       <c r="C55" s="1"/>
@@ -2622,7 +2621,7 @@
     <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A56">
         <f t="shared" ca="1" si="0"/>
-        <v>0.57448281412559032</v>
+        <v>0.20504013956077249</v>
       </c>
       <c r="B56" s="2"/>
       <c r="C56" s="1"/>
@@ -2633,7 +2632,7 @@
     <row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A57">
         <f t="shared" ca="1" si="0"/>
-        <v>0.44290263375997274</v>
+        <v>0.87360447393515295</v>
       </c>
       <c r="B57" s="2"/>
       <c r="C57" s="1"/>
@@ -2644,7 +2643,7 @@
     <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A58">
         <f t="shared" ca="1" si="0"/>
-        <v>0.27787688772250441</v>
+        <v>0.77810448967846835</v>
       </c>
       <c r="B58" s="2"/>
       <c r="C58" s="1"/>
@@ -2655,7 +2654,7 @@
     <row r="59" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A59">
         <f t="shared" ca="1" si="0"/>
-        <v>0.89812850839025615</v>
+        <v>0.59441113452071137</v>
       </c>
       <c r="B59" s="2"/>
       <c r="C59" s="1"/>
@@ -2666,7 +2665,7 @@
     <row r="60" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A60">
         <f t="shared" ca="1" si="0"/>
-        <v>0.96530107076469229</v>
+        <v>0.81087003294455395</v>
       </c>
       <c r="B60" s="2"/>
       <c r="C60" s="1"/>
@@ -2677,7 +2676,7 @@
     <row r="61" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A61">
         <f t="shared" ca="1" si="0"/>
-        <v>0.14176270258879531</v>
+        <v>0.30738062670506305</v>
       </c>
       <c r="B61" s="2"/>
       <c r="C61" s="1"/>
@@ -2696,8 +2695,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5678AB3F-32DD-CA45-8A4B-C8D15816A975}">
   <dimension ref="A1:R40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E34" sqref="E34:E38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2712,41 +2711,41 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="29" t="s">
         <v>113</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="E1" s="23" t="s">
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="E1" s="26" t="s">
         <v>114</v>
       </c>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23"/>
-      <c r="H1" s="23"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="26"/>
       <c r="K1" s="17" t="s">
         <v>83</v>
       </c>
-      <c r="L1" s="28" t="s">
+      <c r="L1" s="31" t="s">
         <v>109</v>
       </c>
-      <c r="M1" s="28"/>
-      <c r="N1" s="28"/>
-      <c r="O1" s="28"/>
-      <c r="P1" s="28"/>
+      <c r="M1" s="31"/>
+      <c r="N1" s="31"/>
+      <c r="O1" s="31"/>
+      <c r="P1" s="31"/>
       <c r="Q1" s="17"/>
       <c r="R1" s="17"/>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A2" s="27"/>
-      <c r="B2" s="27"/>
-      <c r="C2" s="27"/>
-      <c r="E2" s="23"/>
-      <c r="F2" s="23"/>
-      <c r="G2" s="23"/>
-      <c r="H2" s="23"/>
+      <c r="A2" s="30"/>
+      <c r="B2" s="30"/>
+      <c r="C2" s="30"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="26"/>
+      <c r="G2" s="26"/>
+      <c r="H2" s="26"/>
       <c r="K2" s="17"/>
-      <c r="L2" s="25"/>
-      <c r="M2" s="25"/>
+      <c r="L2" s="28"/>
+      <c r="M2" s="28"/>
       <c r="N2" s="17"/>
       <c r="O2" s="17"/>
       <c r="P2" s="17"/>
@@ -2754,13 +2753,13 @@
       <c r="R2" s="17"/>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A3" s="27"/>
-      <c r="B3" s="27"/>
-      <c r="C3" s="27"/>
-      <c r="E3" s="23"/>
-      <c r="F3" s="23"/>
-      <c r="G3" s="23"/>
-      <c r="H3" s="23"/>
+      <c r="A3" s="30"/>
+      <c r="B3" s="30"/>
+      <c r="C3" s="30"/>
+      <c r="E3" s="26"/>
+      <c r="F3" s="26"/>
+      <c r="G3" s="26"/>
+      <c r="H3" s="26"/>
       <c r="K3" s="17" t="s">
         <v>84</v>
       </c>
@@ -2773,13 +2772,13 @@
       <c r="R3" s="17"/>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A4" s="27"/>
-      <c r="B4" s="27"/>
-      <c r="C4" s="27"/>
-      <c r="E4" s="23"/>
-      <c r="F4" s="23"/>
-      <c r="G4" s="23"/>
-      <c r="H4" s="23"/>
+      <c r="A4" s="30"/>
+      <c r="B4" s="30"/>
+      <c r="C4" s="30"/>
+      <c r="E4" s="26"/>
+      <c r="F4" s="26"/>
+      <c r="G4" s="26"/>
+      <c r="H4" s="26"/>
       <c r="K4" s="17" t="s">
         <v>108</v>
       </c>
@@ -2800,18 +2799,18 @@
       <c r="R4" s="17"/>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A5" s="27"/>
-      <c r="B5" s="27"/>
-      <c r="C5" s="27"/>
-      <c r="E5" s="23"/>
-      <c r="F5" s="23"/>
-      <c r="G5" s="23"/>
-      <c r="H5" s="23"/>
+      <c r="A5" s="30"/>
+      <c r="B5" s="30"/>
+      <c r="C5" s="30"/>
+      <c r="E5" s="26"/>
+      <c r="F5" s="26"/>
+      <c r="G5" s="26"/>
+      <c r="H5" s="26"/>
       <c r="K5" s="17" t="s">
         <v>73</v>
       </c>
       <c r="L5" s="17" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="M5" s="17"/>
       <c r="N5" s="17"/>
@@ -2826,23 +2825,23 @@
       <c r="R5" s="17"/>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A6" s="27"/>
-      <c r="B6" s="27"/>
-      <c r="C6" s="27"/>
-      <c r="E6" s="23"/>
-      <c r="F6" s="23"/>
-      <c r="G6" s="23"/>
-      <c r="H6" s="23"/>
+      <c r="A6" s="30"/>
+      <c r="B6" s="30"/>
+      <c r="C6" s="30"/>
+      <c r="E6" s="26"/>
+      <c r="F6" s="26"/>
+      <c r="G6" s="26"/>
+      <c r="H6" s="26"/>
       <c r="K6" s="17" t="s">
         <v>77</v>
       </c>
       <c r="L6" s="17" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="M6" s="17"/>
       <c r="N6" s="17"/>
       <c r="O6" s="17" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="P6" s="17" cm="1">
         <f t="array" ref="P6">MorningGameRowStart</f>
@@ -2852,18 +2851,18 @@
       <c r="R6" s="17"/>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A7" s="27"/>
-      <c r="B7" s="27"/>
-      <c r="C7" s="27"/>
-      <c r="E7" s="23"/>
-      <c r="F7" s="23"/>
-      <c r="G7" s="23"/>
-      <c r="H7" s="23"/>
+      <c r="A7" s="30"/>
+      <c r="B7" s="30"/>
+      <c r="C7" s="30"/>
+      <c r="E7" s="26"/>
+      <c r="F7" s="26"/>
+      <c r="G7" s="26"/>
+      <c r="H7" s="26"/>
       <c r="K7" s="17" t="s">
         <v>81</v>
       </c>
       <c r="L7" s="17" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="M7" s="17"/>
       <c r="N7" s="17"/>
@@ -2873,13 +2872,13 @@
       <c r="R7" s="17"/>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A8" s="27"/>
-      <c r="B8" s="27"/>
-      <c r="C8" s="27"/>
-      <c r="E8" s="23"/>
-      <c r="F8" s="23"/>
-      <c r="G8" s="23"/>
-      <c r="H8" s="23"/>
+      <c r="A8" s="30"/>
+      <c r="B8" s="30"/>
+      <c r="C8" s="30"/>
+      <c r="E8" s="26"/>
+      <c r="F8" s="26"/>
+      <c r="G8" s="26"/>
+      <c r="H8" s="26"/>
       <c r="K8" s="17"/>
       <c r="L8" s="17"/>
       <c r="M8" s="17"/>
@@ -2890,13 +2889,13 @@
       <c r="R8" s="17"/>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A9" s="27"/>
-      <c r="B9" s="27"/>
-      <c r="C9" s="27"/>
-      <c r="E9" s="23"/>
-      <c r="F9" s="23"/>
-      <c r="G9" s="23"/>
-      <c r="H9" s="23"/>
+      <c r="A9" s="30"/>
+      <c r="B9" s="30"/>
+      <c r="C9" s="30"/>
+      <c r="E9" s="26"/>
+      <c r="F9" s="26"/>
+      <c r="G9" s="26"/>
+      <c r="H9" s="26"/>
       <c r="K9" s="17"/>
       <c r="L9" s="17"/>
       <c r="M9" s="17"/>
@@ -2907,13 +2906,13 @@
       <c r="R9" s="17"/>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A10" s="27"/>
-      <c r="B10" s="27"/>
-      <c r="C10" s="27"/>
-      <c r="E10" s="23"/>
-      <c r="F10" s="23"/>
-      <c r="G10" s="23"/>
-      <c r="H10" s="23"/>
+      <c r="A10" s="30"/>
+      <c r="B10" s="30"/>
+      <c r="C10" s="30"/>
+      <c r="E10" s="26"/>
+      <c r="F10" s="26"/>
+      <c r="G10" s="26"/>
+      <c r="H10" s="26"/>
       <c r="K10" s="17"/>
       <c r="L10" s="17"/>
       <c r="M10" s="17"/>
@@ -2924,13 +2923,13 @@
       <c r="R10" s="17"/>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A11" s="27"/>
-      <c r="B11" s="27"/>
-      <c r="C11" s="27"/>
-      <c r="E11" s="23"/>
-      <c r="F11" s="23"/>
-      <c r="G11" s="23"/>
-      <c r="H11" s="23"/>
+      <c r="A11" s="30"/>
+      <c r="B11" s="30"/>
+      <c r="C11" s="30"/>
+      <c r="E11" s="26"/>
+      <c r="F11" s="26"/>
+      <c r="G11" s="26"/>
+      <c r="H11" s="26"/>
       <c r="K11" s="17"/>
       <c r="L11" s="17"/>
       <c r="M11" s="17"/>
@@ -2941,13 +2940,13 @@
       <c r="R11" s="17"/>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A12" s="27"/>
-      <c r="B12" s="27"/>
-      <c r="C12" s="27"/>
-      <c r="E12" s="23"/>
-      <c r="F12" s="23"/>
-      <c r="G12" s="23"/>
-      <c r="H12" s="23"/>
+      <c r="A12" s="30"/>
+      <c r="B12" s="30"/>
+      <c r="C12" s="30"/>
+      <c r="E12" s="26"/>
+      <c r="F12" s="26"/>
+      <c r="G12" s="26"/>
+      <c r="H12" s="26"/>
       <c r="K12" s="17"/>
       <c r="L12" s="17"/>
       <c r="M12" s="17"/>
@@ -2958,13 +2957,13 @@
       <c r="R12" s="17"/>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A13" s="27"/>
-      <c r="B13" s="27"/>
-      <c r="C13" s="27"/>
-      <c r="E13" s="23"/>
-      <c r="F13" s="23"/>
-      <c r="G13" s="23"/>
-      <c r="H13" s="23"/>
+      <c r="A13" s="30"/>
+      <c r="B13" s="30"/>
+      <c r="C13" s="30"/>
+      <c r="E13" s="26"/>
+      <c r="F13" s="26"/>
+      <c r="G13" s="26"/>
+      <c r="H13" s="26"/>
       <c r="K13" s="17"/>
       <c r="L13" s="17"/>
       <c r="M13" s="17"/>
@@ -2975,13 +2974,13 @@
       <c r="R13" s="17"/>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A14" s="27"/>
-      <c r="B14" s="27"/>
-      <c r="C14" s="27"/>
-      <c r="E14" s="23"/>
-      <c r="F14" s="23"/>
-      <c r="G14" s="23"/>
-      <c r="H14" s="23"/>
+      <c r="A14" s="30"/>
+      <c r="B14" s="30"/>
+      <c r="C14" s="30"/>
+      <c r="E14" s="26"/>
+      <c r="F14" s="26"/>
+      <c r="G14" s="26"/>
+      <c r="H14" s="26"/>
       <c r="K14" s="17"/>
       <c r="L14" s="17"/>
       <c r="M14" s="17"/>
@@ -2993,12 +2992,12 @@
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
-        <v>161</v>
-      </c>
-      <c r="E15" s="23"/>
-      <c r="F15" s="23"/>
-      <c r="G15" s="23"/>
-      <c r="H15" s="23"/>
+        <v>160</v>
+      </c>
+      <c r="E15" s="26"/>
+      <c r="F15" s="26"/>
+      <c r="G15" s="26"/>
+      <c r="H15" s="26"/>
       <c r="K15" s="17"/>
       <c r="L15" s="17"/>
       <c r="M15" s="17"/>
@@ -3034,19 +3033,19 @@
         <f>IF(COUNTIF('Team List'!B2:B61,"&lt;&gt;") &lt;=B17*B18,"Enough Judging Slots","Not enough judging slots")</f>
         <v>Enough Judging Slots</v>
       </c>
-      <c r="E17" s="30" t="s">
-        <v>173</v>
+      <c r="E17" s="23" t="s">
+        <v>172</v>
       </c>
       <c r="F17" s="16">
         <v>0.33333333333333331</v>
       </c>
-      <c r="K17" s="25" t="s">
+      <c r="K17" s="28" t="s">
         <v>72</v>
       </c>
-      <c r="L17" s="25"/>
-      <c r="M17" s="25"/>
-      <c r="N17" s="25"/>
-      <c r="O17" s="25"/>
+      <c r="L17" s="28"/>
+      <c r="M17" s="28"/>
+      <c r="N17" s="28"/>
+      <c r="O17" s="28"/>
       <c r="P17" s="17"/>
       <c r="Q17" s="17"/>
       <c r="R17" s="17"/>
@@ -3058,32 +3057,32 @@
       <c r="B18" s="14">
         <v>6</v>
       </c>
-      <c r="E18" s="30" t="s">
-        <v>174</v>
+      <c r="E18" s="23" t="s">
+        <v>173</v>
       </c>
       <c r="F18" s="15">
         <v>4.1666666666666664E-2</v>
       </c>
-      <c r="K18" s="25" t="s">
+      <c r="K18" s="28" t="s">
         <v>82</v>
       </c>
-      <c r="L18" s="25"/>
-      <c r="M18" s="25"/>
-      <c r="N18" s="25"/>
-      <c r="O18" s="25"/>
+      <c r="L18" s="28"/>
+      <c r="M18" s="28"/>
+      <c r="N18" s="28"/>
+      <c r="O18" s="28"/>
       <c r="P18" s="17"/>
       <c r="Q18" s="17"/>
       <c r="R18" s="17"/>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A19" s="32" t="s">
-        <v>176</v>
+      <c r="A19" t="s">
+        <v>175</v>
       </c>
       <c r="B19" s="15">
         <v>2.0833333333333332E-2</v>
       </c>
-      <c r="E19" s="31" t="s">
-        <v>175</v>
+      <c r="E19" s="24" t="s">
+        <v>174</v>
       </c>
       <c r="F19" s="16">
         <v>0.47916666666666669</v>
@@ -3102,8 +3101,8 @@
       <c r="R19" s="17"/>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A20" s="33" t="s">
-        <v>177</v>
+      <c r="A20" s="6" t="s">
+        <v>176</v>
       </c>
       <c r="B20" s="15">
         <v>1.0416666666666666E-2</v>
@@ -3134,8 +3133,8 @@
       <c r="C21" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="E21" s="29" t="s">
-        <v>171</v>
+      <c r="E21" s="22" t="s">
+        <v>170</v>
       </c>
       <c r="F21" s="16">
         <v>0.33333333333333331</v>
@@ -3146,21 +3145,21 @@
         <v>0</v>
       </c>
       <c r="N21" s="17" t="str">
-        <f>CONCATENATE($G$25," A")</f>
+        <f>CONCATENATE($E$35," A")</f>
         <v>Red A</v>
       </c>
       <c r="O21" s="18">
         <v>0</v>
       </c>
       <c r="P21" s="17" t="str">
-        <f>CONCATENATE($G$25," B")</f>
+        <f>CONCATENATE($E$35," B")</f>
         <v>Red B</v>
       </c>
       <c r="Q21" s="18">
         <v>0</v>
       </c>
       <c r="R21" s="17" t="str">
-        <f>CONCATENATE($G$25," A")</f>
+        <f>CONCATENATE($E$35," A")</f>
         <v>Red A</v>
       </c>
     </row>
@@ -3174,8 +3173,8 @@
       <c r="C22" s="16">
         <v>0.375</v>
       </c>
-      <c r="E22" s="29" t="s">
-        <v>172</v>
+      <c r="E22" s="22" t="s">
+        <v>171</v>
       </c>
       <c r="F22" s="16">
         <v>0.33333333333333331</v>
@@ -3186,21 +3185,21 @@
         <v>0</v>
       </c>
       <c r="N22" s="17" t="str">
-        <f>CONCATENATE($G$25," B")</f>
+        <f>CONCATENATE($E$35," B")</f>
         <v>Red B</v>
       </c>
       <c r="O22" s="18">
         <v>0</v>
       </c>
       <c r="P22" s="17" t="str">
-        <f>CONCATENATE($G$25," A")</f>
+        <f>CONCATENATE($E$35," A")</f>
         <v>Red A</v>
       </c>
       <c r="Q22" s="18">
         <v>0</v>
       </c>
       <c r="R22" s="17" t="str">
-        <f>CONCATENATE($G$25," B")</f>
+        <f>CONCATENATE($E$35," B")</f>
         <v>Red B</v>
       </c>
     </row>
@@ -3221,7 +3220,7 @@
         <v>2</v>
       </c>
       <c r="G23" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="K23" s="17"/>
       <c r="L23" s="17"/>
@@ -3248,9 +3247,6 @@
       <c r="F24" s="14">
         <v>1</v>
       </c>
-      <c r="G24" s="6" t="s">
-        <v>71</v>
-      </c>
       <c r="K24" s="17" t="s">
         <v>77</v>
       </c>
@@ -3280,9 +3276,6 @@
       <c r="F25" s="15">
         <v>3.472222222222222E-3</v>
       </c>
-      <c r="G25" s="14" t="s">
-        <v>53</v>
-      </c>
       <c r="K25" s="17"/>
       <c r="L25" s="17"/>
       <c r="M25" s="18"/>
@@ -3309,13 +3302,10 @@
         <v>0.5625</v>
       </c>
       <c r="E26" s="6" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F26" s="16">
         <v>0.375</v>
-      </c>
-      <c r="G26" s="14" t="s">
-        <v>41</v>
       </c>
       <c r="K26" s="17"/>
       <c r="L26" s="17"/>
@@ -3323,7 +3313,7 @@
         <v>0</v>
       </c>
       <c r="N26" s="17" t="str">
-        <f>CONCATENATE($G$25," A")</f>
+        <f>CONCATENATE($E$35," A")</f>
         <v>Red A</v>
       </c>
       <c r="O26" s="18">
@@ -3331,14 +3321,14 @@
         <v>3.472222222222222E-3</v>
       </c>
       <c r="P26" s="17" t="str">
-        <f>CONCATENATE($G$26," B")</f>
+        <f>CONCATENATE($E$36," B")</f>
         <v>Blue B</v>
       </c>
       <c r="Q26" s="18">
         <v>0</v>
       </c>
       <c r="R26" s="17" t="str">
-        <f>CONCATENATE($G$25," B")</f>
+        <f>CONCATENATE($E$35," B")</f>
         <v>Red B</v>
       </c>
     </row>
@@ -3353,13 +3343,10 @@
         <v>0.60416666666666663</v>
       </c>
       <c r="E27" s="6" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="F27" s="16">
         <v>0.4375</v>
-      </c>
-      <c r="G27" s="14" t="s">
-        <v>40</v>
       </c>
       <c r="K27" s="17"/>
       <c r="L27" s="17"/>
@@ -3367,14 +3354,14 @@
         <v>0</v>
       </c>
       <c r="N27" s="17" t="str">
-        <f>CONCATENATE($G$25," B")</f>
+        <f>CONCATENATE($E$35," B")</f>
         <v>Red B</v>
       </c>
       <c r="O27" s="18">
         <v>0</v>
       </c>
       <c r="P27" s="17" t="str">
-        <f>CONCATENATE($G$25," A")</f>
+        <f>CONCATENATE($E$35," A")</f>
         <v>Red A</v>
       </c>
       <c r="Q27" s="18">
@@ -3382,7 +3369,7 @@
         <v>3.472222222222222E-3</v>
       </c>
       <c r="R27" s="17" t="str">
-        <f>CONCATENATE($G$26," A")</f>
+        <f>CONCATENATE($E$36," A")</f>
         <v>Blue A</v>
       </c>
     </row>
@@ -3395,13 +3382,10 @@
       </c>
       <c r="C28" s="11"/>
       <c r="E28" s="6" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="F28" s="16">
         <v>0.44791666666666669</v>
-      </c>
-      <c r="G28" s="14" t="s">
-        <v>54</v>
       </c>
       <c r="K28" s="17"/>
       <c r="L28" s="17"/>
@@ -3410,21 +3394,21 @@
         <v>3.472222222222222E-3</v>
       </c>
       <c r="N28" s="17" t="str">
-        <f>CONCATENATE($G$26," A")</f>
+        <f>CONCATENATE($E$36," A")</f>
         <v>Blue A</v>
       </c>
       <c r="O28" s="18">
         <v>0</v>
       </c>
       <c r="P28" s="17" t="str">
-        <f>CONCATENATE($G$25," B")</f>
+        <f>CONCATENATE($E$35," B")</f>
         <v>Red B</v>
       </c>
       <c r="Q28" s="18">
         <v>0</v>
       </c>
       <c r="R28" s="17" t="str">
-        <f>CONCATENATE($G$25," A")</f>
+        <f>CONCATENATE($E$35," A")</f>
         <v>Red A</v>
       </c>
     </row>
@@ -3437,7 +3421,7 @@
       </c>
       <c r="C29" s="11"/>
       <c r="E29" s="6" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F29" s="16">
         <v>0.52083333333333337</v>
@@ -3449,7 +3433,7 @@
         <v>3.472222222222222E-3</v>
       </c>
       <c r="N29" s="17" t="str">
-        <f>CONCATENATE($G$26," B")</f>
+        <f>CONCATENATE($E$36," B")</f>
         <v>Blue B</v>
       </c>
       <c r="O29" s="18">
@@ -3457,7 +3441,7 @@
         <v>3.472222222222222E-3</v>
       </c>
       <c r="P29" s="17" t="str">
-        <f>CONCATENATE($G$26," A")</f>
+        <f>CONCATENATE($E$36," A")</f>
         <v>Blue A</v>
       </c>
       <c r="Q29" s="18">
@@ -3465,7 +3449,7 @@
         <v>3.472222222222222E-3</v>
       </c>
       <c r="R29" s="17" t="str">
-        <f>CONCATENATE($G$26," B")</f>
+        <f>CONCATENATE($E$36," B")</f>
         <v>Blue B</v>
       </c>
     </row>
@@ -3477,7 +3461,7 @@
         <v>110</v>
       </c>
       <c r="E30" s="6" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F30" s="16">
         <v>0.52083333333333337</v>
@@ -3499,7 +3483,7 @@
         <v>110</v>
       </c>
       <c r="E31" s="6" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="F31" s="16">
         <v>0.5625</v>
@@ -3519,7 +3503,7 @@
     </row>
     <row r="32" spans="1:18" x14ac:dyDescent="0.2">
       <c r="E32" s="6" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="F32" s="16">
         <v>0.5625</v>
@@ -3541,7 +3525,7 @@
     </row>
     <row r="33" spans="5:18" x14ac:dyDescent="0.2">
       <c r="E33" s="6" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="F33" s="16">
         <v>0.60416666666666663</v>
@@ -3552,7 +3536,7 @@
         <v>0</v>
       </c>
       <c r="N33" s="17" t="str">
-        <f>CONCATENATE($G$25," A")</f>
+        <f>CONCATENATE($E$35," A")</f>
         <v>Red A</v>
       </c>
       <c r="O33" s="18">
@@ -3560,32 +3544,35 @@
         <v>3.472222222222222E-3</v>
       </c>
       <c r="P33" s="17" t="str">
-        <f>CONCATENATE($G$26," B")</f>
+        <f>CONCATENATE($E$36," B")</f>
         <v>Blue B</v>
       </c>
       <c r="Q33" s="18">
         <v>0</v>
       </c>
       <c r="R33" s="17" t="str">
-        <f>CONCATENATE($G$25," B")</f>
+        <f>CONCATENATE($E$35," B")</f>
         <v>Red B</v>
       </c>
     </row>
     <row r="34" spans="5:18" x14ac:dyDescent="0.2">
+      <c r="E34" s="6" t="s">
+        <v>71</v>
+      </c>
       <c r="K34" s="17"/>
       <c r="L34" s="17"/>
       <c r="M34" s="18">
         <v>0</v>
       </c>
       <c r="N34" s="17" t="str">
-        <f>CONCATENATE($G$25," B")</f>
+        <f>CONCATENATE($E$35," B")</f>
         <v>Red B</v>
       </c>
       <c r="O34" s="18">
         <v>0</v>
       </c>
       <c r="P34" s="17" t="str">
-        <f>CONCATENATE($G$25," A")</f>
+        <f>CONCATENATE($E$35," A")</f>
         <v>Red A</v>
       </c>
       <c r="Q34" s="18">
@@ -3593,11 +3580,14 @@
         <v>3.472222222222222E-3</v>
       </c>
       <c r="R34" s="17" t="str">
-        <f>CONCATENATE($G$26," A")</f>
+        <f>CONCATENATE($E$36," A")</f>
         <v>Blue A</v>
       </c>
     </row>
     <row r="35" spans="5:18" x14ac:dyDescent="0.2">
+      <c r="E35" s="14" t="s">
+        <v>53</v>
+      </c>
       <c r="K35" s="17"/>
       <c r="L35" s="17"/>
       <c r="M35" s="18">
@@ -3605,25 +3595,28 @@
         <v>3.472222222222222E-3</v>
       </c>
       <c r="N35" s="17" t="str">
-        <f>CONCATENATE($G$26," A")</f>
+        <f>CONCATENATE($E$36," A")</f>
         <v>Blue A</v>
       </c>
       <c r="O35" s="18">
         <v>0</v>
       </c>
       <c r="P35" s="17" t="str">
-        <f>CONCATENATE($G$25," B")</f>
+        <f>CONCATENATE($E$35," B")</f>
         <v>Red B</v>
       </c>
       <c r="Q35" s="18">
         <v>0</v>
       </c>
       <c r="R35" s="17" t="str">
-        <f>CONCATENATE($G$25," A")</f>
+        <f>CONCATENATE($E$35," A")</f>
         <v>Red A</v>
       </c>
     </row>
     <row r="36" spans="5:18" x14ac:dyDescent="0.2">
+      <c r="E36" s="14" t="s">
+        <v>41</v>
+      </c>
       <c r="K36" s="17"/>
       <c r="L36" s="17"/>
       <c r="M36" s="18">
@@ -3631,7 +3624,7 @@
         <v>3.472222222222222E-3</v>
       </c>
       <c r="N36" s="17" t="str">
-        <f>CONCATENATE($G$26," B")</f>
+        <f>CONCATENATE($E$36," B")</f>
         <v>Blue B</v>
       </c>
       <c r="O36" s="18">
@@ -3639,7 +3632,7 @@
         <v>3.472222222222222E-3</v>
       </c>
       <c r="P36" s="17" t="str">
-        <f>CONCATENATE($G$26," A")</f>
+        <f>CONCATENATE($E$36," A")</f>
         <v>Blue A</v>
       </c>
       <c r="Q36" s="18">
@@ -3647,11 +3640,14 @@
         <v>3.472222222222222E-3</v>
       </c>
       <c r="R36" s="17" t="str">
-        <f>CONCATENATE($G$26," B")</f>
+        <f>CONCATENATE($E$36," B")</f>
         <v>Blue B</v>
       </c>
     </row>
     <row r="37" spans="5:18" x14ac:dyDescent="0.2">
+      <c r="E37" s="14" t="s">
+        <v>40</v>
+      </c>
       <c r="K37" s="17"/>
       <c r="L37" s="17"/>
       <c r="M37" s="18">
@@ -3659,7 +3655,7 @@
         <v>6.9444444444444441E-3</v>
       </c>
       <c r="N37" s="17" t="str">
-        <f>CONCATENATE($G$27," A")</f>
+        <f>CONCATENATE($E$37," A")</f>
         <v>Green A</v>
       </c>
       <c r="O37" s="18">
@@ -3667,7 +3663,7 @@
         <v>1.0416666666666666E-2</v>
       </c>
       <c r="P37" s="17" t="str">
-        <f>CONCATENATE($G$28," B")</f>
+        <f>CONCATENATE($E$38," B")</f>
         <v>Purple B</v>
       </c>
       <c r="Q37" s="18">
@@ -3675,11 +3671,14 @@
         <v>6.9444444444444441E-3</v>
       </c>
       <c r="R37" s="17" t="str">
-        <f>CONCATENATE($G$27," B")</f>
+        <f>CONCATENATE($E$37," B")</f>
         <v>Green B</v>
       </c>
     </row>
     <row r="38" spans="5:18" x14ac:dyDescent="0.2">
+      <c r="E38" s="14" t="s">
+        <v>54</v>
+      </c>
       <c r="K38" s="17"/>
       <c r="L38" s="17"/>
       <c r="M38" s="18">
@@ -3687,7 +3686,7 @@
         <v>6.9444444444444441E-3</v>
       </c>
       <c r="N38" s="17" t="str">
-        <f>CONCATENATE($G$27," B")</f>
+        <f>CONCATENATE($E$37," B")</f>
         <v>Green B</v>
       </c>
       <c r="O38" s="18">
@@ -3695,7 +3694,7 @@
         <v>6.9444444444444441E-3</v>
       </c>
       <c r="P38" s="17" t="str">
-        <f>CONCATENATE($G$27," A")</f>
+        <f>CONCATENATE($E$37," A")</f>
         <v>Green A</v>
       </c>
       <c r="Q38" s="18">
@@ -3703,7 +3702,7 @@
         <v>1.0416666666666666E-2</v>
       </c>
       <c r="R38" s="17" t="str">
-        <f>CONCATENATE($G$28," A")</f>
+        <f>CONCATENATE($E$38," A")</f>
         <v>Purple A</v>
       </c>
     </row>
@@ -3715,7 +3714,7 @@
         <v>1.0416666666666666E-2</v>
       </c>
       <c r="N39" s="17" t="str">
-        <f>CONCATENATE($G$28," A")</f>
+        <f>CONCATENATE($E$38," A")</f>
         <v>Purple A</v>
       </c>
       <c r="O39" s="18">
@@ -3723,7 +3722,7 @@
         <v>6.9444444444444441E-3</v>
       </c>
       <c r="P39" s="17" t="str">
-        <f>CONCATENATE($G$27," B")</f>
+        <f>CONCATENATE($E$37," B")</f>
         <v>Green B</v>
       </c>
       <c r="Q39" s="18">
@@ -3731,7 +3730,7 @@
         <v>6.9444444444444441E-3</v>
       </c>
       <c r="R39" s="17" t="str">
-        <f>CONCATENATE($G$27," A")</f>
+        <f>CONCATENATE($E$37," A")</f>
         <v>Green A</v>
       </c>
     </row>
@@ -3743,7 +3742,7 @@
         <v>1.0416666666666666E-2</v>
       </c>
       <c r="N40" s="17" t="str">
-        <f>CONCATENATE($G$28," B")</f>
+        <f>CONCATENATE($E$38," B")</f>
         <v>Purple B</v>
       </c>
       <c r="O40" s="18">
@@ -3751,7 +3750,7 @@
         <v>1.0416666666666666E-2</v>
       </c>
       <c r="P40" s="17" t="str">
-        <f>CONCATENATE($G$28," A")</f>
+        <f>CONCATENATE($E$38," A")</f>
         <v>Purple A</v>
       </c>
       <c r="Q40" s="18">
@@ -3759,7 +3758,7 @@
         <v>1.0416666666666666E-2</v>
       </c>
       <c r="R40" s="17" t="str">
-        <f>CONCATENATE($G$28," B")</f>
+        <f>CONCATENATE($E$38," B")</f>
         <v>Purple B</v>
       </c>
     </row>
@@ -3793,8 +3792,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8A29ECE-34EE-4F45-8C40-B65CFF553BC6}">
   <dimension ref="A1:Q74"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18:XFD18"/>
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6285,7 +6284,7 @@
   <dimension ref="A1:AG61"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A39" sqref="A39"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -14514,10 +14513,10 @@
         <v>44869</v>
       </c>
       <c r="B4" t="s">
+        <v>146</v>
+      </c>
+      <c r="C4" t="s">
         <v>147</v>
-      </c>
-      <c r="C4" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -14525,10 +14524,10 @@
         <v>44869</v>
       </c>
       <c r="B5" t="s">
+        <v>148</v>
+      </c>
+      <c r="C5" t="s">
         <v>149</v>
-      </c>
-      <c r="C5" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -14536,10 +14535,10 @@
         <v>44869</v>
       </c>
       <c r="B6" t="s">
+        <v>150</v>
+      </c>
+      <c r="C6" t="s">
         <v>151</v>
-      </c>
-      <c r="C6" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
@@ -14547,10 +14546,10 @@
         <v>44902</v>
       </c>
       <c r="B7" t="s">
+        <v>161</v>
+      </c>
+      <c r="C7" t="s">
         <v>162</v>
-      </c>
-      <c r="C7" t="s">
-        <v>163</v>
       </c>
     </row>
   </sheetData>
@@ -14563,7 +14562,7 @@
   <dimension ref="A1:O241"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B62" sqref="B62"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -14576,35 +14575,35 @@
         <v>50</v>
       </c>
       <c r="B1" t="s">
+        <v>152</v>
+      </c>
+      <c r="C1" t="s">
         <v>153</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>154</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>155</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>156</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>157</v>
-      </c>
-      <c r="G1" t="s">
-        <v>158</v>
       </c>
       <c r="H1" t="s">
         <v>0</v>
       </c>
       <c r="L1" s="20" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="M1" s="20"/>
       <c r="N1" s="20" t="s">
+        <v>158</v>
+      </c>
+      <c r="O1" s="20" t="s">
         <v>159</v>
-      </c>
-      <c r="O1" s="20" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="2" spans="1:15" ht="16" x14ac:dyDescent="0.2">

</xml_diff>